<commit_message>
Aggiornato RAD e SDD
Matrice di tracciabilità nel RAD (aggiungere nell'indice e collegamento)
SDD aggiunta tabella modifiche
</commit_message>
<xml_diff>
--- a/Documenti/RAD/Matrice/Matrice di Tracciabilità.xlsx
+++ b/Documenti/RAD/Matrice/Matrice di Tracciabilità.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afuci\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adri9\OneDrive\Documenti\GitHub\FRAA\Documenti\RAD\Matrice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D267E82-A024-478E-A76C-4DFBB819213C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40A7B94-1E2B-4B15-9416-40630B97E98E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9E4AE140-89A6-48C9-A358-C6F247045042}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>Nome Progeto:</t>
   </si>
   <si>
-    <t>MeedQueue</t>
-  </si>
-  <si>
     <t>Descrizione del progetto:</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>MedQueue</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
   <dimension ref="B2:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B2" sqref="B2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,22 +687,22 @@
       </c>
       <c r="C2" s="4"/>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4"/>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -710,81 +710,81 @@
     </row>
     <row r="7" spans="2:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="O7" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -792,37 +792,37 @@
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -830,37 +830,37 @@
     </row>
     <row r="10" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -868,37 +868,37 @@
     </row>
     <row r="11" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -906,45 +906,170 @@
     </row>
     <row r="12" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="2:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="8:15" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="26" spans="8:15" x14ac:dyDescent="0.25">
       <c r="O26" s="6"/>
     </row>
   </sheetData>

</xml_diff>